<commit_message>
LeverettJ + new optimal scale
Push changes before adding imperm cells.
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8351a88428b982e/Master/MRST/summer_sintef/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{5A7E1129-02B9-4081-9DC3-4B1F6E6D9705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA00C491-86FB-4B03-A152-7D061D0F5354}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="8_{5A7E1129-02B9-4081-9DC3-4B1F6E6D9705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE98E791-80C6-43B7-AA68-2EE6178FD54F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EA72C794-5F15-4919-A5C6-0FE572CB2F79}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="55">
   <si>
     <t>nr layers</t>
   </si>
@@ -156,12 +156,6 @@
     <t>Case 4 - study 1 (pc)</t>
   </si>
   <si>
-    <t>[50, 100]</t>
-  </si>
-  <si>
-    <t>[600, 600]</t>
-  </si>
-  <si>
     <t>12 m^3/s</t>
   </si>
   <si>
@@ -174,15 +168,9 @@
     <t>p_e</t>
   </si>
   <si>
-    <t>1*barsa</t>
-  </si>
-  <si>
     <t>p_cap</t>
   </si>
   <si>
-    <t>5*barsa</t>
-  </si>
-  <si>
     <t>std_gauss</t>
   </si>
   <si>
@@ -190,6 +178,27 @@
   </si>
   <si>
     <t>corr_len_z</t>
+  </si>
+  <si>
+    <t>poro</t>
+  </si>
+  <si>
+    <t>[75, 75]</t>
+  </si>
+  <si>
+    <t>0.5*barsa</t>
+  </si>
+  <si>
+    <t>3*barsa</t>
+  </si>
+  <si>
+    <t>[800, 450]</t>
+  </si>
+  <si>
+    <t>lowperm</t>
+  </si>
+  <si>
+    <t>20 md</t>
   </si>
 </sst>
 </file>
@@ -548,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5DEDC5-385B-4572-A390-E60F8AFF0B4D}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -913,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -921,7 +930,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -929,7 +938,7 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -937,7 +946,7 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -945,7 +954,7 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -974,23 +983,23 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B26">
         <v>0.8</v>
@@ -998,7 +1007,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B27">
         <v>200</v>
@@ -1006,10 +1015,26 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B28">
         <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>